<commit_message>
added land expectation to the pipeline
</commit_message>
<xml_diff>
--- a/WorkingData/Spreadsheets/testme.xlsx
+++ b/WorkingData/Spreadsheets/testme.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,7 +496,12 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Land Price (R per Ha</t>
+          <t>Land Price (R per Ha)</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Total Land Price (R)</t>
         </is>
       </c>
     </row>
@@ -551,6 +556,9 @@
       <c r="N2" t="n">
         <v>6212.595318060035</v>
       </c>
+      <c r="O2" t="n">
+        <v>72247782.81229447</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -603,6 +611,9 @@
       <c r="N3" t="n">
         <v>3097.995045655855</v>
       </c>
+      <c r="O3" t="n">
+        <v>20782635.09843159</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -655,6 +666,9 @@
       <c r="N4" t="n">
         <v>5120.483717816567</v>
       </c>
+      <c r="O4" t="n">
+        <v>22593800.7240546</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -707,6 +721,9 @@
       <c r="N5" t="n">
         <v>13106.04868300527</v>
       </c>
+      <c r="O5" t="n">
+        <v>232581616.7967931</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -759,6 +776,9 @@
       <c r="N6" t="n">
         <v>13140.32384288267</v>
       </c>
+      <c r="O6" t="n">
+        <v>464676097.8206922</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -811,6 +831,9 @@
       <c r="N7" t="n">
         <v>2675.291446150483</v>
       </c>
+      <c r="O7" t="n">
+        <v>20853736.30525625</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -863,6 +886,9 @@
       <c r="N8" t="n">
         <v>5827.844472153663</v>
       </c>
+      <c r="O8" t="n">
+        <v>62319368.09302074</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -915,6 +941,9 @@
       <c r="N9" t="n">
         <v>5700.752980229388</v>
       </c>
+      <c r="O9" t="n">
+        <v>37765179.12383224</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -965,6 +994,9 @@
       <c r="N10" t="n">
         <v>13050.30136414688</v>
       </c>
+      <c r="O10" t="n">
+        <v>242233887.2037748</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1017,6 +1049,9 @@
       <c r="N11" t="n">
         <v>4735.42619024193</v>
       </c>
+      <c r="O11" t="n">
+        <v>31183721.91838449</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1069,6 +1104,9 @@
       <c r="N12" t="n">
         <v>13240.47679873659</v>
       </c>
+      <c r="O12" t="n">
+        <v>222864603.1357782</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1121,6 +1159,9 @@
       <c r="N13" t="n">
         <v>469.889041114775</v>
       </c>
+      <c r="O13" t="n">
+        <v>3779931.300469709</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1173,6 +1214,9 @@
       <c r="N14" t="n">
         <v>3409.935999805508</v>
       </c>
+      <c r="O14" t="n">
+        <v>33320255.08831654</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1225,6 +1269,9 @@
       <c r="N15" t="n">
         <v>5640.682702004432</v>
       </c>
+      <c r="O15" t="n">
+        <v>56768718.01137516</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1277,6 +1324,9 @@
       <c r="N16" t="n">
         <v>2663.903952400452</v>
       </c>
+      <c r="O16" t="n">
+        <v>24373193.11248379</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1329,6 +1379,9 @@
       <c r="N17" t="n">
         <v>5142.124670180133</v>
       </c>
+      <c r="O17" t="n">
+        <v>47322808.09180501</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1381,6 +1434,9 @@
       <c r="N18" t="n">
         <v>5943.308271895984</v>
       </c>
+      <c r="O18" t="n">
+        <v>63706712.53960895</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1433,6 +1489,9 @@
       <c r="N19" t="n">
         <v>13081.89823098832</v>
       </c>
+      <c r="O19" t="n">
+        <v>430793046.6636483</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1485,6 +1544,9 @@
       <c r="N20" t="n">
         <v>3447.982145311837</v>
       </c>
+      <c r="O20" t="n">
+        <v>29484760.20079239</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1537,6 +1599,9 @@
       <c r="N21" t="n">
         <v>2576.220791038358</v>
       </c>
+      <c r="O21" t="n">
+        <v>13662971.44586958</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1589,6 +1654,9 @@
       <c r="N22" t="n">
         <v>5973.357975894152</v>
       </c>
+      <c r="O22" t="n">
+        <v>52989783.04911486</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1641,6 +1709,9 @@
       <c r="N23" t="n">
         <v>2568.528617943771</v>
       </c>
+      <c r="O23" t="n">
+        <v>15037271.59408078</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1693,6 +1764,9 @@
       <c r="N24" t="n">
         <v>13157.69473838931</v>
       </c>
+      <c r="O24" t="n">
+        <v>265968968.6051389</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1745,6 +1819,9 @@
       <c r="N25" t="n">
         <v>3524.304524259554</v>
       </c>
+      <c r="O25" t="n">
+        <v>91725669.25305666</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1797,6 +1874,9 @@
       <c r="N26" t="n">
         <v>13050.30136414688</v>
       </c>
+      <c r="O26" t="n">
+        <v>534393842.7625261</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1849,6 +1929,9 @@
       <c r="N27" t="n">
         <v>5004.945694740944</v>
       </c>
+      <c r="O27" t="n">
+        <v>70222983.77083158</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1900,6 +1983,9 @@
       </c>
       <c r="N28" t="n">
         <v>4562.767947752509</v>
+      </c>
+      <c r="O28" t="n">
+        <v>33296145.17918894</v>
       </c>
     </row>
   </sheetData>

</xml_diff>